<commit_message>
Added test files; coded filed translate
</commit_message>
<xml_diff>
--- a/ingester-server/src/test/resources/sqlqueries/MappingSheetInserts.xlsx
+++ b/ingester-server/src/test/resources/sqlqueries/MappingSheetInserts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x049709/Documentos/Ingester Project Files/sqlqueries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x049709/Documentos/Git Projects/ingester-server/src/test/resources/sqlqueries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D28DB8-B626-4D41-853E-8C777136B3C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D372FBE-275B-C643-BE66-42163FB805F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="206">
   <si>
     <t>SOURCE_ENTITY</t>
   </si>
@@ -5037,10 +5037,6 @@
   </si>
   <si>
     <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
-values ('LOC','TYPE','inField007','LOC','TYPE','Y','DECIMAL');</t>
-  </si>
-  <si>
-    <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
 values ('LOC','ALTPLANTID','inField008','LOC','ALTPLANTID','Y','NONE');</t>
   </si>
   <si>
@@ -5097,10 +5093,6 @@
   </si>
   <si>
     <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
-values ('LOC','COUNTRY','inField024','LOC','COUNTRY','N','NONE');</t>
-  </si>
-  <si>
-    <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
 values ('LOC','CURRENCY','inField025','LOC','CURRENCY','N','NONE');</t>
   </si>
   <si>
@@ -5181,6 +5173,20 @@
   <si>
     <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
 values ('LOC','SEQINTLASTIMPORTEDFROMSEQ','inField022','LOC','SEQINTLASTIMPORTEDFROMSEQ','N','DATE');</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
+  </si>
+  <si>
+    <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
+values ('LOC','TYPE','inField007','LOC','TYPE','Y','INTEGER');</t>
+  </si>
+  <si>
+    <t>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
+values ('LOC','COUNTRY','inField024','LOC','COUNTRY','N','LOOKUP');</t>
   </si>
 </sst>
 </file>
@@ -6058,8 +6064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6229,7 +6235,7 @@
         <v>159</v>
       </c>
       <c r="K4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>161</v>
@@ -6240,7 +6246,7 @@
 values ('LOC','OHPOST','inField003','LOC','OHPOST','Y','DATE');</v>
       </c>
       <c r="N4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6275,7 +6281,7 @@
         <v>159</v>
       </c>
       <c r="K5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>161</v>
@@ -6286,7 +6292,7 @@
 values ('LOC','FRZSTART','inField004','LOC','FRZSTART','Y','DATE');</v>
       </c>
       <c r="N5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6413,7 +6419,7 @@
         <v>159</v>
       </c>
       <c r="K8" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>161</v>
@@ -6421,10 +6427,10 @@
       <c r="M8" t="str">
         <f t="shared" si="0"/>
         <v>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
-values ('LOC','TYPE','inField007','LOC','TYPE','Y','DECIMAL');</v>
+values ('LOC','TYPE','inField007','LOC','TYPE','Y','INTEGER');</v>
       </c>
       <c r="N8" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6470,7 +6476,7 @@
 values ('LOC','ALTPLANTID','inField008','LOC','ALTPLANTID','Y','NONE');</v>
       </c>
       <c r="N9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6516,7 +6522,7 @@
 values ('LOC','CUST','inField009','LOC','CUST','Y','NONE');</v>
       </c>
       <c r="N10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6562,7 +6568,7 @@
 values ('LOC','TRANSZONE','inField010','LOC','TRANSZONE','Y','NONE');</v>
       </c>
       <c r="N11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6608,7 +6614,7 @@
 values ('LOC','LAT','inField011','LOC','LAT','Y','DECIMAL');</v>
       </c>
       <c r="N12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6654,7 +6660,7 @@
 values ('LOC','LON','inField012','LOC','LON','Y','DECIMAL');</v>
       </c>
       <c r="N13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6700,7 +6706,7 @@
 values ('LOC','ENABLESW','inField013','LOC','ENABLESW','Y','DECIMAL');</v>
       </c>
       <c r="N14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6746,7 +6752,7 @@
 values ('LOC','FF_TRIGGER_CONTROL','inField014','LOC','FF_TRIGGER_CONTROL','Y','DECIMAL');</v>
       </c>
       <c r="N15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6792,7 +6798,7 @@
 values ('LOC','LOC_TYPE','inField015','LOC','LOC_TYPE','Y','NONE');</v>
       </c>
       <c r="N16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6838,7 +6844,7 @@
 values ('LOC','VENDID','inField016','LOC','VENDID','Y','NONE');</v>
       </c>
       <c r="N17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6884,7 +6890,7 @@
 values ('LOC','COMPANYID','inField017','LOC','COMPANYID','Y','NONE');</v>
       </c>
       <c r="N18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6930,7 +6936,7 @@
 values ('LOC','WORKINGCAL','inField018','LOC','WORKINGCAL','Y','NONE');</v>
       </c>
       <c r="N19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6976,7 +6982,7 @@
 values ('LOC','SEQINTEXPORTDUR','inField019','LOC','SEQINTEXPORTDUR','N','DECIMAL');</v>
       </c>
       <c r="N20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7022,7 +7028,7 @@
 values ('LOC','SEQINTIMPORTDUR','inField020','LOC','SEQINTIMPORTDUR','N','DECIMAL');</v>
       </c>
       <c r="N21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7057,7 +7063,7 @@
         <v>160</v>
       </c>
       <c r="K22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>161</v>
@@ -7068,7 +7074,7 @@
 values ('LOC','SEQINTLASTEXPORTEDTOSEQ','inField021','LOC','SEQINTLASTEXPORTEDTOSEQ','N','DATE');</v>
       </c>
       <c r="N22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7103,7 +7109,7 @@
         <v>160</v>
       </c>
       <c r="K23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>161</v>
@@ -7114,7 +7120,7 @@
 values ('LOC','SEQINTLASTIMPORTEDFROMSEQ','inField022','LOC','SEQINTLASTIMPORTEDFROMSEQ','N','DATE');</v>
       </c>
       <c r="N23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7160,7 +7166,7 @@
 values ('LOC','POSTALCODE','inField023','LOC','POSTALCODE','N','NONE');</v>
       </c>
       <c r="N24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7195,7 +7201,7 @@
         <v>160</v>
       </c>
       <c r="K25" t="s">
-        <v>11</v>
+        <v>203</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>161</v>
@@ -7203,10 +7209,10 @@
       <c r="M25" t="str">
         <f t="shared" si="0"/>
         <v>insert into SalesLt.MappingSheet (SOURCE_ENTITY, SOURCE_COL_NAME, GENERIC_COL_NAME, TARGET_ENTITY, TARGET_COL_NAME, REQUIRED_FLAG,INGESTION_RULE) 
-values ('LOC','COUNTRY','inField024','LOC','COUNTRY','N','NONE');</v>
+values ('LOC','COUNTRY','inField024','LOC','COUNTRY','N','LOOKUP');</v>
       </c>
       <c r="N25" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7252,7 +7258,7 @@
 values ('LOC','CURRENCY','inField025','LOC','CURRENCY','N','NONE');</v>
       </c>
       <c r="N26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7298,7 +7304,7 @@
 values ('LOC','WDDAREA','inField026','LOC','WDDAREA','N','NONE');</v>
       </c>
       <c r="N27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7344,7 +7350,7 @@
 values ('LOC','BORROWINGPCT','inField027','LOC','BORROWINGPCT','N','DECIMAL');</v>
       </c>
       <c r="N28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7390,7 +7396,7 @@
 values ('LOC','HIERARCHYLEVEL','inField028','LOC','HIERARCHYLEVEL','N','NONE');</v>
       </c>
       <c r="N29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7436,7 +7442,7 @@
 values ('LOC','ORDERCOST','inField029','LOC','ORDERCOST','N','DECIMAL');</v>
       </c>
       <c r="N30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7482,7 +7488,7 @@
 values ('LOC','SOURCELOC','inField030','LOC','SOURCELOC','N','NONE');</v>
       </c>
       <c r="N31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7528,7 +7534,7 @@
 values ('LOC','U_NATIONLOCATIONID','inField031','LOC','U_NATIONLOCATIONID','N','NONE');</v>
       </c>
       <c r="N32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7574,7 +7580,7 @@
 values ('LOC','U_PROFILE_DESIGNATION','inField032','LOC','U_PROFILE_DESIGNATION','Y','NONE');</v>
       </c>
       <c r="N33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7620,7 +7626,7 @@
 values ('LOC','U_ETHNICITY','inField033','LOC','U_ETHNICITY','Y','NONE');</v>
       </c>
       <c r="N34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7666,7 +7672,7 @@
 values ('LOC','U_CORP_VOLUME_GROUP','inField034','LOC','U_CORP_VOLUME_GROUP','Y','NONE');</v>
       </c>
       <c r="N35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7712,7 +7718,7 @@
 values ('LOC','U_SCHOOL_START_WK','inField035','LOC','U_SCHOOL_START_WK','Y','NONE');</v>
       </c>
       <c r="N36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7758,7 +7764,7 @@
 values ('LOC','U_TOURIST_FLAG','inField036','LOC','U_TOURIST_FLAG','Y','NONE');</v>
       </c>
       <c r="N37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7804,7 +7810,7 @@
 values ('LOC','U_COLD_SUMMER','inField037','LOC','U_COLD_SUMMER','Y','NONE');</v>
       </c>
       <c r="N38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7850,7 +7856,7 @@
 values ('LOC','U_WARM_WEATHER','inField038','LOC','U_WARM_WEATHER','Y','NONE');</v>
       </c>
       <c r="N39" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7896,7 +7902,7 @@
 values ('LOC','U_EXTREME_GROWTH','inField039','LOC','U_EXTREME_GROWTH','N','NONE');</v>
       </c>
       <c r="N40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -7942,7 +7948,7 @@
 values ('LOC','U_CER_STORE','inField040','LOC','U_CER_STORE','N','NONE');</v>
       </c>
       <c r="N41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>